<commit_message>
Update xlsx example sheet.
</commit_message>
<xml_diff>
--- a/README/MATH/Positions_Calculations.xlsx
+++ b/README/MATH/Positions_Calculations.xlsx
@@ -8,12 +8,13 @@
     <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
     <sheet name="Scenario 1 - Initial Subsidy in" sheetId="2" r:id="rId5"/>
     <sheet name="Scenario 2 - DON'T INCLDUE Init" sheetId="3" r:id="rId6"/>
+    <sheet name="Scenario 3 - Edge Case Transact" sheetId="4" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -169,6 +170,15 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>Scenario 3 - Edge Case Transactions - Divide By Zero</t>
+  </si>
+  <si>
+    <t>Scenario 3 - Edge Case Transact</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -359,7 +369,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -442,6 +452,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1558,6 +1571,22 @@
         <v>49</v>
       </c>
     </row>
+    <row r="13">
+      <c r="B13" t="s" s="3">
+        <v>52</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="4"/>
+      <c r="C14" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s" s="5">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
@@ -1565,6 +1594,7 @@
   <hyperlinks>
     <hyperlink ref="D10" location="'Scenario 1 - Initial Subsidy in'!R2C1" tooltip="" display="Scenario 1 - Initial Subsidy in"/>
     <hyperlink ref="D12" location="'Scenario 2 - DON''T INCLDUE Init'!R2C1" tooltip="" display="Scenario 2 - DON'T INCLDUE Init"/>
+    <hyperlink ref="D14" location="'Scenario 3 - Edge Case Transact'!R2C1" tooltip="" display="Scenario 3 - Edge Case Transact"/>
   </hyperlinks>
 </worksheet>
 </file>
@@ -3062,7 +3092,8 @@
     <col min="17" max="19" width="4.50781" style="28" customWidth="1"/>
     <col min="20" max="20" width="6.57812" style="28" customWidth="1"/>
     <col min="21" max="21" width="5.72656" style="28" customWidth="1"/>
-    <col min="22" max="27" width="4.50781" style="28" customWidth="1"/>
+    <col min="22" max="26" width="5.73438" style="28" customWidth="1"/>
+    <col min="27" max="27" width="4.50781" style="28" customWidth="1"/>
     <col min="28" max="28" width="8.8125" style="28" customWidth="1"/>
     <col min="29" max="30" width="9.57812" style="28" customWidth="1"/>
     <col min="31" max="31" width="11.2188" style="28" customWidth="1"/>
@@ -3160,7 +3191,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" ht="152.25" customHeight="1">
+    <row r="3" ht="128.25" customHeight="1">
       <c r="A3" t="s" s="10">
         <v>10</v>
       </c>
@@ -3367,15 +3398,17 @@
         <v>0.166666666666667</v>
       </c>
       <c r="J5" s="23"/>
-      <c r="K5" s="24">
-        <f>D5*I5</f>
-        <v>3.33333333333334</v>
-      </c>
-      <c r="L5" s="24">
-        <f>D5*(1-I5)</f>
-        <v>16.6666666666667</v>
-      </c>
-      <c r="M5" s="24"/>
+      <c r="K5" s="25">
+        <f>ROUND(D5*I5,0)</f>
+        <v>3</v>
+      </c>
+      <c r="L5" s="25">
+        <f>ROUND(D5*(1-I5),0)</f>
+        <v>17</v>
+      </c>
+      <c r="M5" s="24">
+        <v>0</v>
+      </c>
       <c r="N5" s="24"/>
       <c r="O5" s="24"/>
       <c r="P5" s="24"/>
@@ -3437,13 +3470,13 @@
         <v>0.375</v>
       </c>
       <c r="J6" s="23"/>
-      <c r="K6" s="24">
-        <f>D6*I6</f>
-        <v>11.25</v>
-      </c>
-      <c r="L6" s="24">
-        <f>D6*(1-I6)</f>
-        <v>18.75</v>
+      <c r="K6" s="25">
+        <f>ROUND(D6*I6,0)</f>
+        <v>11</v>
+      </c>
+      <c r="L6" s="25">
+        <f>ROUND(D6*(1-I6),0)</f>
+        <v>19</v>
       </c>
       <c r="M6" s="22">
         <f>ABS($I6-$I$5)*$B$5</f>
@@ -3469,7 +3502,7 @@
       </c>
       <c r="U6" s="22">
         <f>L6/S6</f>
-        <v>4.50000000000001</v>
+        <v>4.56000000000001</v>
       </c>
       <c r="V6" s="25">
         <f>ROUND(M6*U6,0)</f>
@@ -3556,12 +3589,12 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="23"/>
-      <c r="K7" s="24">
-        <f>D7*I7</f>
+      <c r="K7" s="25">
+        <f>ROUND(D7*I7,0)</f>
         <v>20</v>
       </c>
-      <c r="L7" s="24">
-        <f>D7*(1-I7)</f>
+      <c r="L7" s="25">
+        <f>ROUND(D7*(1-I7),0)</f>
         <v>20</v>
       </c>
       <c r="M7" s="22">
@@ -3685,13 +3718,13 @@
         <v>0.625</v>
       </c>
       <c r="J8" s="23"/>
-      <c r="K8" s="24">
-        <f>D8*I8</f>
-        <v>18.75</v>
-      </c>
-      <c r="L8" s="24">
-        <f>D8*(1-I8)</f>
-        <v>11.25</v>
+      <c r="K8" s="25">
+        <f>ROUND(D8*I8,0)</f>
+        <v>19</v>
+      </c>
+      <c r="L8" s="25">
+        <f>ROUND(D8*(1-I8),0)</f>
+        <v>11</v>
       </c>
       <c r="M8" s="22">
         <f>ABS(I8-$I$5)*$B$5</f>
@@ -3720,11 +3753,11 @@
       </c>
       <c r="T8" s="22">
         <f>K8/R8</f>
-        <v>5</v>
+        <v>5.06666666666667</v>
       </c>
       <c r="U8" s="22">
         <f>L8/S8</f>
-        <v>1.22727272727273</v>
+        <v>1.2</v>
       </c>
       <c r="V8" s="25">
         <f>ROUND(M8*U8,0)</f>
@@ -3823,13 +3856,13 @@
         <v>0.785714285714286</v>
       </c>
       <c r="J9" s="23"/>
-      <c r="K9" s="24">
-        <f>D9*I9</f>
-        <v>47.1428571428572</v>
-      </c>
-      <c r="L9" s="24">
-        <f>D9*(1-I9)</f>
-        <v>12.8571428571428</v>
+      <c r="K9" s="25">
+        <f>ROUND(D9*I9,0)</f>
+        <v>47</v>
+      </c>
+      <c r="L9" s="25">
+        <f>ROUND(D9*(1-I9),0)</f>
+        <v>13</v>
       </c>
       <c r="M9" s="22">
         <f>ABS(I9-$I$5)*$B$5</f>
@@ -3861,11 +3894,11 @@
       </c>
       <c r="T9" s="22">
         <f>K9/R9</f>
-        <v>6.76923076923077</v>
+        <v>6.74871794871794</v>
       </c>
       <c r="U9" s="22">
         <f>L9/S9</f>
-        <v>1.19337016574585</v>
+        <v>1.20662983425415</v>
       </c>
       <c r="V9" s="25">
         <f>ROUND(M9*U9,0)</f>
@@ -4544,4 +4577,1526 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A2:AM24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="B4" xSplit="1" ySplit="3" activePane="bottomRight" state="frozen"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="14.9297" style="29" customWidth="1"/>
+    <col min="2" max="2" width="10.5859" style="29" customWidth="1"/>
+    <col min="3" max="3" width="11.9609" style="29" customWidth="1"/>
+    <col min="4" max="8" width="3.625" style="29" customWidth="1"/>
+    <col min="9" max="9" width="5.72656" style="29" customWidth="1"/>
+    <col min="10" max="10" width="3.34375" style="29" customWidth="1"/>
+    <col min="11" max="12" width="6.85156" style="29" customWidth="1"/>
+    <col min="13" max="14" width="4.17969" style="29" customWidth="1"/>
+    <col min="15" max="15" width="3.89844" style="29" customWidth="1"/>
+    <col min="16" max="16" width="3.58594" style="29" customWidth="1"/>
+    <col min="17" max="19" width="4.50781" style="29" customWidth="1"/>
+    <col min="20" max="20" width="6.57812" style="29" customWidth="1"/>
+    <col min="21" max="21" width="5.72656" style="29" customWidth="1"/>
+    <col min="22" max="27" width="4.50781" style="29" customWidth="1"/>
+    <col min="28" max="28" width="8.8125" style="29" customWidth="1"/>
+    <col min="29" max="30" width="9.57812" style="29" customWidth="1"/>
+    <col min="31" max="31" width="11.2188" style="29" customWidth="1"/>
+    <col min="32" max="39" width="9.59375" style="29" customWidth="1"/>
+    <col min="40" max="16384" width="16.3516" style="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="27.65" customHeight="1">
+      <c r="A1" t="s" s="7">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+    </row>
+    <row r="2" ht="68.05" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" t="s" s="9">
+        <v>7</v>
+      </c>
+      <c r="AF2" t="s" s="9">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="AL2" t="s" s="9">
+        <v>50</v>
+      </c>
+      <c r="AM2" s="8"/>
+    </row>
+    <row r="3" ht="152.25" customHeight="1">
+      <c r="A3" t="s" s="10">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s" s="10">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s" s="10">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="10">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s" s="10">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s" s="10">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s" s="10">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s" s="10">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s" s="10">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="L3" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s" s="10">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s" s="10">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s" s="10">
+        <v>24</v>
+      </c>
+      <c r="P3" t="s" s="10">
+        <v>25</v>
+      </c>
+      <c r="Q3" t="s" s="10">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s" s="10">
+        <v>27</v>
+      </c>
+      <c r="S3" t="s" s="10">
+        <v>28</v>
+      </c>
+      <c r="T3" t="s" s="10">
+        <v>29</v>
+      </c>
+      <c r="U3" t="s" s="10">
+        <v>30</v>
+      </c>
+      <c r="V3" t="s" s="10">
+        <v>31</v>
+      </c>
+      <c r="W3" t="s" s="10">
+        <v>32</v>
+      </c>
+      <c r="X3" t="s" s="10">
+        <v>33</v>
+      </c>
+      <c r="Y3" t="s" s="10">
+        <v>34</v>
+      </c>
+      <c r="Z3" t="s" s="10">
+        <v>35</v>
+      </c>
+      <c r="AA3" t="s" s="10">
+        <v>36</v>
+      </c>
+      <c r="AB3" t="s" s="10">
+        <v>37</v>
+      </c>
+      <c r="AC3" t="s" s="10">
+        <v>38</v>
+      </c>
+      <c r="AD3" t="s" s="10">
+        <v>39</v>
+      </c>
+      <c r="AE3" s="11"/>
+      <c r="AF3" t="s" s="10">
+        <v>40</v>
+      </c>
+      <c r="AG3" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="AH3" t="s" s="10">
+        <v>42</v>
+      </c>
+      <c r="AI3" t="s" s="10">
+        <v>43</v>
+      </c>
+      <c r="AJ3" t="s" s="10">
+        <v>44</v>
+      </c>
+      <c r="AK3" s="11"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+    </row>
+    <row r="4" ht="20.25" customHeight="1">
+      <c r="A4" s="12">
+        <v>0</v>
+      </c>
+      <c r="B4" s="13">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s" s="14">
+        <v>45</v>
+      </c>
+      <c r="D4" s="15">
+        <v>0</v>
+      </c>
+      <c r="E4" s="15">
+        <f>COUNTIF(B4:C4,"YES")</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="15">
+        <f>COUNTIF(C4:D4,"NO")</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="15">
+        <f>B4*E4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="15">
+        <f>B4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="17"/>
+      <c r="AJ4" s="17"/>
+      <c r="AK4" s="17"/>
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="17"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" s="18">
+        <v>1</v>
+      </c>
+      <c r="B5" s="19">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s" s="20">
+        <v>46</v>
+      </c>
+      <c r="D5" s="21">
+        <f>D4+B5</f>
+        <v>10</v>
+      </c>
+      <c r="E5" s="21">
+        <f>COUNTIF(B5:C5,"YES")</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="21">
+        <f>COUNTIF(C5:D5,"NO")</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="21">
+        <f>G4+B5*E5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="21">
+        <f>H4+B5*F5</f>
+        <v>10</v>
+      </c>
+      <c r="I5" s="22">
+        <f>($B$4*$I$4+G5)/($B$4+G5+H5)</f>
+        <v>0.25</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="25">
+        <f>ROUND(D5*I5,0)</f>
+        <v>3</v>
+      </c>
+      <c r="L5" s="25">
+        <f>ROUND(D5*(1-I5),0)</f>
+        <v>8</v>
+      </c>
+      <c r="M5" s="24">
+        <v>0</v>
+      </c>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="24"/>
+      <c r="AJ5" s="24"/>
+      <c r="AK5" s="24"/>
+      <c r="AL5" s="24"/>
+      <c r="AM5" s="24"/>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="18">
+        <v>2</v>
+      </c>
+      <c r="B6" s="19">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="D6" s="21">
+        <f>D5+B6</f>
+        <v>15</v>
+      </c>
+      <c r="E6" s="21">
+        <f>COUNTIF(B6:C6,"YES")</f>
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
+        <f>COUNTIF(C6:D6,"NO")</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="21">
+        <f>G5+B6*E6</f>
+        <v>5</v>
+      </c>
+      <c r="H6" s="21">
+        <f>H5+B6*F6</f>
+        <v>10</v>
+      </c>
+      <c r="I6" s="22">
+        <f>($B$4*$I$4+G6)/($B$4+G6+H6)</f>
+        <v>0.4</v>
+      </c>
+      <c r="J6" s="23"/>
+      <c r="K6" s="25">
+        <f>ROUND(D6*I6,0)</f>
+        <v>6</v>
+      </c>
+      <c r="L6" s="25">
+        <f>ROUND(D6*(1-I6),0)</f>
+        <v>9</v>
+      </c>
+      <c r="M6" s="22">
+        <f>ABS($I6-$I$5)*$B$5</f>
+        <v>1.5</v>
+      </c>
+      <c r="N6" s="22">
+        <f>ABS($I6-$I$6)*$B$6</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="22">
+        <f>N6+O6+Q6</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="22">
+        <f>M6+P6</f>
+        <v>1.5</v>
+      </c>
+      <c r="T6" s="22">
+        <v>0</v>
+      </c>
+      <c r="U6" s="22">
+        <f>L6/S6</f>
+        <v>6</v>
+      </c>
+      <c r="V6" s="25">
+        <f>ROUND(M6*U6,0)</f>
+        <v>9</v>
+      </c>
+      <c r="W6" s="25">
+        <f>ROUND(N6*T6,0)</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="24">
+        <f>SUM(V6:Z6)</f>
+        <v>9</v>
+      </c>
+      <c r="AB6" s="25">
+        <f>AA6-D6</f>
+        <v>-6</v>
+      </c>
+      <c r="AC6" t="b" s="21">
+        <f>AB6&gt;0</f>
+        <v>0</v>
+      </c>
+      <c r="AD6" t="b" s="21">
+        <f>AB6&lt;0</f>
+        <v>1</v>
+      </c>
+      <c r="AE6" s="24">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="25">
+        <f>ROUNDDOWN(ABS(AB6)/2,0)+1+V6</f>
+        <v>13</v>
+      </c>
+      <c r="AG6" s="25">
+        <f>ROUNDDOWN(ABS(AB6)/2,0)+W6</f>
+        <v>3</v>
+      </c>
+      <c r="AH6" s="23"/>
+      <c r="AI6" s="23"/>
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="25">
+        <f>SUM(AF6:AJ6)</f>
+        <v>16</v>
+      </c>
+      <c r="AL6" t="s" s="20">
+        <f>IF(D6=AK6,"TRUE","FALSE")</f>
+        <v>54</v>
+      </c>
+      <c r="AM6" s="23"/>
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" s="18">
+        <v>3</v>
+      </c>
+      <c r="B7" s="19">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="D7" s="21">
+        <f>D6+B7</f>
+        <v>20</v>
+      </c>
+      <c r="E7" s="21">
+        <f>COUNTIF(B7:C7,"YES")</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="21">
+        <f>COUNTIF(C7:D7,"NO")</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="21">
+        <f>G6+B7*E7</f>
+        <v>10</v>
+      </c>
+      <c r="H7" s="21">
+        <f>H6+B7*F7</f>
+        <v>10</v>
+      </c>
+      <c r="I7" s="22">
+        <f>($B$4*$I$4+G7)/($B$4+G7+H7)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="23"/>
+      <c r="K7" s="25">
+        <f>ROUND(D7*I7,0)</f>
+        <v>10</v>
+      </c>
+      <c r="L7" s="25">
+        <f>ROUND(D7*(1-I7),0)</f>
+        <v>10</v>
+      </c>
+      <c r="M7" s="22">
+        <f>ABS(I7-$I$5)*$B$5</f>
+        <v>2.5</v>
+      </c>
+      <c r="N7" s="22">
+        <f>ABS($I7-$I$6)*$B$6</f>
+        <v>0.5</v>
+      </c>
+      <c r="O7" s="22">
+        <f>ABS($I7-$I$7)*$B$7</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="22">
+        <f>N7+O7+Q7</f>
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="22">
+        <f>M7+P7</f>
+        <v>2.5</v>
+      </c>
+      <c r="T7" s="22">
+        <f>K7/R7</f>
+        <v>20</v>
+      </c>
+      <c r="U7" s="22">
+        <f>L7/S7</f>
+        <v>4</v>
+      </c>
+      <c r="V7" s="25">
+        <f>ROUND(M7*U7,0)</f>
+        <v>10</v>
+      </c>
+      <c r="W7" s="25">
+        <f>ROUND(N7*T7,0)</f>
+        <v>10</v>
+      </c>
+      <c r="X7" s="25">
+        <f>ROUND(O7*T7,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="24">
+        <f>SUM(V7:Z7)</f>
+        <v>20</v>
+      </c>
+      <c r="AB7" s="25">
+        <f>AA7-D7</f>
+        <v>0</v>
+      </c>
+      <c r="AC7" t="b" s="21">
+        <f>AB7&gt;0</f>
+        <v>0</v>
+      </c>
+      <c r="AD7" t="b" s="21">
+        <f>AB7&lt;0</f>
+        <v>0</v>
+      </c>
+      <c r="AE7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="25">
+        <f>V7</f>
+        <v>10</v>
+      </c>
+      <c r="AG7" s="25">
+        <f>W7</f>
+        <v>10</v>
+      </c>
+      <c r="AH7" s="25">
+        <f>X7</f>
+        <v>0</v>
+      </c>
+      <c r="AI7" s="23"/>
+      <c r="AJ7" s="23"/>
+      <c r="AK7" s="25">
+        <f>SUM(AF7:AJ7)</f>
+        <v>20</v>
+      </c>
+      <c r="AL7" t="s" s="20">
+        <f>IF(D7=AK7,"TRUE","FALSE")</f>
+        <v>51</v>
+      </c>
+      <c r="AM7" s="23"/>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" s="18">
+        <v>4</v>
+      </c>
+      <c r="B8" s="19">
+        <v>-10</v>
+      </c>
+      <c r="C8" t="s" s="20">
+        <v>46</v>
+      </c>
+      <c r="D8" s="21">
+        <f>D7+B8</f>
+        <v>10</v>
+      </c>
+      <c r="E8" s="21">
+        <f>COUNTIF(B8:C8,"YES")</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="21">
+        <f>COUNTIF(C8:D8,"NO")</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="21">
+        <f>G7+B8*E8</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="21">
+        <f>H7+B8*F8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="22">
+        <f>($B$4*$I$4+G8)/($B$4+G8+H8)</f>
+        <v>0.75</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="25">
+        <f>ROUND(D8*I8,0)</f>
+        <v>8</v>
+      </c>
+      <c r="L8" s="25">
+        <f>ROUND(D8*(1-I8),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M8" s="22">
+        <f>ABS(I8-$I$5)*$B$5</f>
+        <v>5</v>
+      </c>
+      <c r="N8" s="22">
+        <f>ABS($I8-$I$6)*$B$6</f>
+        <v>1.75</v>
+      </c>
+      <c r="O8" s="22">
+        <f>ABS($I8-$I$7)*$B$7</f>
+        <v>1.25</v>
+      </c>
+      <c r="P8" s="22">
+        <f>ABS($I8-$I$8)*$B$8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="24"/>
+      <c r="R8" s="22">
+        <f>N8+O8+Q8</f>
+        <v>3</v>
+      </c>
+      <c r="S8" s="22">
+        <f>M8+P8</f>
+        <v>5</v>
+      </c>
+      <c r="T8" s="22">
+        <f>K8/R8</f>
+        <v>2.66666666666667</v>
+      </c>
+      <c r="U8" s="22">
+        <f>L8/S8</f>
+        <v>0.6</v>
+      </c>
+      <c r="V8" s="25">
+        <f>ROUND(M8*U8,0)</f>
+        <v>3</v>
+      </c>
+      <c r="W8" s="25">
+        <f>ROUND(N8*T8,0)</f>
+        <v>5</v>
+      </c>
+      <c r="X8" s="25">
+        <f>ROUND(O8*T8,0)</f>
+        <v>3</v>
+      </c>
+      <c r="Y8" s="25">
+        <f>ROUND(P8*U8,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="24">
+        <f>SUM(V8:Z8)</f>
+        <v>11</v>
+      </c>
+      <c r="AB8" s="25">
+        <f>AA8-D8</f>
+        <v>1</v>
+      </c>
+      <c r="AC8" t="b" s="21">
+        <f>AB8&gt;0</f>
+        <v>1</v>
+      </c>
+      <c r="AD8" t="b" s="21">
+        <f>AB8&lt;0</f>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="24">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="25">
+        <f>V8</f>
+        <v>3</v>
+      </c>
+      <c r="AG8" s="25">
+        <f>W8</f>
+        <v>5</v>
+      </c>
+      <c r="AH8" s="25">
+        <f>X8-1</f>
+        <v>2</v>
+      </c>
+      <c r="AI8" s="25">
+        <f>Y8</f>
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="25">
+        <f>SUM(AF8:AJ8)</f>
+        <v>10</v>
+      </c>
+      <c r="AL8" t="s" s="20">
+        <f>IF(D8=AK8,"TRUE","FALSE")</f>
+        <v>51</v>
+      </c>
+      <c r="AM8" s="23"/>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" s="18">
+        <v>5</v>
+      </c>
+      <c r="B9" s="19">
+        <v>-10</v>
+      </c>
+      <c r="C9" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="D9" s="21">
+        <f>D8+B9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="21">
+        <f>COUNTIF(B9:C9,"YES")</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="21">
+        <f>COUNTIF(C9:D9,"NO")</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="21">
+        <f>G8+B9*E9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="21">
+        <f>H8+B9*F9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="22">
+        <f>($B$4*$I$4+G9)/($B$4+G9+H9)</f>
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="23"/>
+      <c r="K9" s="25">
+        <f>ROUND(D9*I9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="25">
+        <f>ROUND(D9*(1-I9),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="22">
+        <f>ABS(I9-$I$5)*$B$5</f>
+        <v>2.5</v>
+      </c>
+      <c r="N9" s="22">
+        <f>ABS($I9-$I$6)*$B$6</f>
+        <v>0.5</v>
+      </c>
+      <c r="O9" s="22">
+        <f>ABS($I9-$I$7)*$B$7</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="22">
+        <f>ABS($I9-$I$8)*$B$8</f>
+        <v>-2.5</v>
+      </c>
+      <c r="Q9" s="22">
+        <f>ABS($I9-$I$9)*$B$9</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="22">
+        <f>N9+O9+Q9</f>
+        <v>0.5</v>
+      </c>
+      <c r="S9" s="22">
+        <f>M9+P9</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="22">
+        <f>K9/R9</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="22">
+        <f>L9/S9</f>
+      </c>
+      <c r="V9" s="25">
+        <f>ROUND(M9*U9,0)</f>
+      </c>
+      <c r="W9" s="25">
+        <f>ROUND(N9*T9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="25">
+        <f>ROUND(O9*T9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="25">
+        <f>ROUND(P9*U9,0)</f>
+      </c>
+      <c r="Z9" s="25">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="24">
+        <f>SUM(V9:Z9)</f>
+      </c>
+      <c r="AB9" s="25">
+        <f>AA9-D9</f>
+      </c>
+      <c r="AC9" s="23">
+        <f>AB9&gt;0</f>
+      </c>
+      <c r="AD9" s="23">
+        <f>AB9&lt;0</f>
+      </c>
+      <c r="AE9" s="24">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="25">
+        <f>V9</f>
+      </c>
+      <c r="AG9" s="25">
+        <f>W9</f>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="25">
+        <f>X9</f>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="25">
+        <f>Y9</f>
+      </c>
+      <c r="AJ9" s="25">
+        <f>Z9</f>
+        <v>0</v>
+      </c>
+      <c r="AK9" s="25">
+        <f>SUM(AF9:AJ9)</f>
+      </c>
+      <c r="AL9" s="23">
+        <f>IF(D9=AK9,"TRUE","FALSE")</f>
+      </c>
+      <c r="AM9" s="23"/>
+    </row>
+    <row r="10" ht="20.05" customHeight="1">
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="23"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="23"/>
+      <c r="AA10" s="23"/>
+      <c r="AB10" s="23"/>
+      <c r="AC10" s="23"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="23"/>
+      <c r="AF10" s="23"/>
+      <c r="AG10" s="23"/>
+      <c r="AH10" s="23"/>
+      <c r="AI10" s="23"/>
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="23"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
+    </row>
+    <row r="11" ht="20.05" customHeight="1">
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="23"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="23"/>
+      <c r="AA11" s="23"/>
+      <c r="AB11" s="23"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="23"/>
+      <c r="AE11" s="23"/>
+      <c r="AF11" s="23"/>
+      <c r="AG11" s="23"/>
+      <c r="AH11" s="23"/>
+      <c r="AI11" s="23"/>
+      <c r="AJ11" s="23"/>
+      <c r="AK11" s="23"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
+    </row>
+    <row r="12" ht="20.05" customHeight="1">
+      <c r="A12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+      <c r="AA12" s="23"/>
+      <c r="AB12" s="23"/>
+      <c r="AC12" s="23"/>
+      <c r="AD12" s="23"/>
+      <c r="AE12" s="23"/>
+      <c r="AF12" s="23"/>
+      <c r="AG12" s="23"/>
+      <c r="AH12" s="23"/>
+      <c r="AI12" s="23"/>
+      <c r="AJ12" s="23"/>
+      <c r="AK12" s="23"/>
+      <c r="AL12" s="23"/>
+      <c r="AM12" s="23"/>
+    </row>
+    <row r="13" ht="20.05" customHeight="1">
+      <c r="A13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="23"/>
+      <c r="AC13" s="23"/>
+      <c r="AD13" s="23"/>
+      <c r="AE13" s="23"/>
+      <c r="AF13" s="23"/>
+      <c r="AG13" s="23"/>
+      <c r="AH13" s="23"/>
+      <c r="AI13" s="23"/>
+      <c r="AJ13" s="23"/>
+      <c r="AK13" s="23"/>
+      <c r="AL13" s="23"/>
+      <c r="AM13" s="23"/>
+    </row>
+    <row r="14" ht="20.05" customHeight="1">
+      <c r="A14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="23"/>
+      <c r="AB14" s="23"/>
+      <c r="AC14" s="23"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="23"/>
+      <c r="AF14" s="23"/>
+      <c r="AG14" s="23"/>
+      <c r="AH14" s="23"/>
+      <c r="AI14" s="23"/>
+      <c r="AJ14" s="23"/>
+      <c r="AK14" s="23"/>
+      <c r="AL14" s="23"/>
+      <c r="AM14" s="23"/>
+    </row>
+    <row r="15" ht="20.05" customHeight="1">
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+      <c r="AA15" s="23"/>
+      <c r="AB15" s="23"/>
+      <c r="AC15" s="23"/>
+      <c r="AD15" s="23"/>
+      <c r="AE15" s="23"/>
+      <c r="AF15" s="23"/>
+      <c r="AG15" s="23"/>
+      <c r="AH15" s="23"/>
+      <c r="AI15" s="23"/>
+      <c r="AJ15" s="23"/>
+      <c r="AK15" s="23"/>
+      <c r="AL15" s="23"/>
+      <c r="AM15" s="23"/>
+    </row>
+    <row r="16" ht="20.05" customHeight="1">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
+      <c r="AA16" s="23"/>
+      <c r="AB16" s="23"/>
+      <c r="AC16" s="23"/>
+      <c r="AD16" s="23"/>
+      <c r="AE16" s="23"/>
+      <c r="AF16" s="23"/>
+      <c r="AG16" s="23"/>
+      <c r="AH16" s="23"/>
+      <c r="AI16" s="23"/>
+      <c r="AJ16" s="23"/>
+      <c r="AK16" s="23"/>
+      <c r="AL16" s="23"/>
+      <c r="AM16" s="23"/>
+    </row>
+    <row r="17" ht="20.05" customHeight="1">
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+      <c r="AA17" s="23"/>
+      <c r="AB17" s="23"/>
+      <c r="AC17" s="23"/>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="23"/>
+      <c r="AF17" s="23"/>
+      <c r="AG17" s="23"/>
+      <c r="AH17" s="23"/>
+      <c r="AI17" s="23"/>
+      <c r="AJ17" s="23"/>
+      <c r="AK17" s="23"/>
+      <c r="AL17" s="23"/>
+      <c r="AM17" s="23"/>
+    </row>
+    <row r="18" ht="20.05" customHeight="1">
+      <c r="A18" s="26"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
+      <c r="AA18" s="23"/>
+      <c r="AB18" s="23"/>
+      <c r="AC18" s="23"/>
+      <c r="AD18" s="23"/>
+      <c r="AE18" s="23"/>
+      <c r="AF18" s="23"/>
+      <c r="AG18" s="23"/>
+      <c r="AH18" s="23"/>
+      <c r="AI18" s="23"/>
+      <c r="AJ18" s="23"/>
+      <c r="AK18" s="23"/>
+      <c r="AL18" s="23"/>
+      <c r="AM18" s="23"/>
+    </row>
+    <row r="19" ht="20.05" customHeight="1">
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="23"/>
+      <c r="AG19" s="23"/>
+      <c r="AH19" s="23"/>
+      <c r="AI19" s="23"/>
+      <c r="AJ19" s="23"/>
+      <c r="AK19" s="23"/>
+      <c r="AL19" s="23"/>
+      <c r="AM19" s="23"/>
+    </row>
+    <row r="20" ht="20.05" customHeight="1">
+      <c r="A20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
+      <c r="S20" s="23"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="23"/>
+      <c r="V20" s="23"/>
+      <c r="W20" s="23"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="23"/>
+      <c r="AG20" s="23"/>
+      <c r="AH20" s="23"/>
+      <c r="AI20" s="23"/>
+      <c r="AJ20" s="23"/>
+      <c r="AK20" s="23"/>
+      <c r="AL20" s="23"/>
+      <c r="AM20" s="23"/>
+    </row>
+    <row r="21" ht="20.05" customHeight="1">
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+      <c r="AA21" s="23"/>
+      <c r="AB21" s="23"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="23"/>
+      <c r="AE21" s="23"/>
+      <c r="AF21" s="23"/>
+      <c r="AG21" s="23"/>
+      <c r="AH21" s="23"/>
+      <c r="AI21" s="23"/>
+      <c r="AJ21" s="23"/>
+      <c r="AK21" s="23"/>
+      <c r="AL21" s="23"/>
+      <c r="AM21" s="23"/>
+    </row>
+    <row r="22" ht="20.05" customHeight="1">
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
+      <c r="AE22" s="23"/>
+      <c r="AF22" s="23"/>
+      <c r="AG22" s="23"/>
+      <c r="AH22" s="23"/>
+      <c r="AI22" s="23"/>
+      <c r="AJ22" s="23"/>
+      <c r="AK22" s="23"/>
+      <c r="AL22" s="23"/>
+      <c r="AM22" s="23"/>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="23"/>
+      <c r="V23" s="23"/>
+      <c r="W23" s="23"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+      <c r="AA23" s="23"/>
+      <c r="AB23" s="23"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="23"/>
+      <c r="AF23" s="23"/>
+      <c r="AG23" s="23"/>
+      <c r="AH23" s="23"/>
+      <c r="AI23" s="23"/>
+      <c r="AJ23" s="23"/>
+      <c r="AK23" s="23"/>
+      <c r="AL23" s="23"/>
+      <c r="AM23" s="23"/>
+    </row>
+    <row r="24" ht="20.05" customHeight="1">
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="23"/>
+      <c r="AB24" s="23"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="23"/>
+      <c r="AE24" s="23"/>
+      <c r="AF24" s="23"/>
+      <c r="AG24" s="23"/>
+      <c r="AH24" s="23"/>
+      <c r="AI24" s="23"/>
+      <c r="AJ24" s="23"/>
+      <c r="AK24" s="23"/>
+      <c r="AL24" s="23"/>
+      <c r="AM24" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:AM1"/>
+  </mergeCells>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>